<commit_message>
ajout des fichiers sql actualisés
</commit_message>
<xml_diff>
--- a/sql/guitaresSAE301.xlsx
+++ b/sql/guitaresSAE301.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\natha\Documents\tout\taf\univ\BUTMMI\MMI2\S3\SAE301\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\natha\Documents\tout\taf\univ\BUTMMI\MMI2\S3\SAE301\sql\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DCD2E65-22EE-42D7-8E5D-556293084FE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF83EB3B-C04B-4CD7-A8E1-E81CFF95F1DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{B7EEBC87-74D8-4820-A7B1-D836DE95E624}"/>
+    <workbookView xWindow="11355" yWindow="1140" windowWidth="24015" windowHeight="8085" xr2:uid="{B7EEBC87-74D8-4820-A7B1-D836DE95E624}"/>
   </bookViews>
   <sheets>
     <sheet name="Table instru" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="674" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="695" uniqueCount="204">
   <si>
     <t>reference</t>
   </si>
@@ -570,9 +570,6 @@
     <t>SKU448CharcoalBurst</t>
   </si>
   <si>
-    <t>nomimage</t>
-  </si>
-  <si>
     <t>idmagasin</t>
   </si>
   <si>
@@ -592,6 +589,72 @@
   </si>
   <si>
     <t>stock</t>
+  </si>
+  <si>
+    <t>nomImage</t>
+  </si>
+  <si>
+    <t>Music Passion 87</t>
+  </si>
+  <si>
+    <t>26 Av. des Bénédictins</t>
+  </si>
+  <si>
+    <t>Le magasin de musique de Limoges. Une large gamme de guitares acoustiques, électriques, électro-ac mais aussi de basses, pianos, claviers et batteries.</t>
+  </si>
+  <si>
+    <t>FNAC Limoges</t>
+  </si>
+  <si>
+    <t>8 Rue des Combes BP 30190</t>
+  </si>
+  <si>
+    <t>Située dans le centre-ville de Limoges, la Fnac vous accueille dans son magasin d’une superficie de plus de 2100m2. Vous y retrouverez tous les univers de la Fnac : livres, disques, DVD, micro‐informatique, objets connectés, gaming, téléphonie, son, photo, TV, papeterie,… Pour vos places de spectacles l’espace billetterie de Fnac Spectacles propose une large sélection d’événements.</t>
+  </si>
+  <si>
+    <t>Cultura Limoges</t>
+  </si>
+  <si>
+    <t>30 Rue Amédée Gordini</t>
+  </si>
+  <si>
+    <t>Cultura enseigne leader de biens de loisirs culturels et créatifs</t>
+  </si>
+  <si>
+    <t>Music Mania</t>
+  </si>
+  <si>
+    <t>12 Rue Jules Guesde</t>
+  </si>
+  <si>
+    <t>Petit magasin proposant un large eventail de produits</t>
+  </si>
+  <si>
+    <t>5 Rue de la Glâne, 87000 Limoges</t>
+  </si>
+  <si>
+    <t>5 Rue de la Glâne</t>
+  </si>
+  <si>
+    <t>Limouzik</t>
+  </si>
+  <si>
+    <t>rien</t>
+  </si>
+  <si>
+    <t>45.832950, 1.267190</t>
+  </si>
+  <si>
+    <t>45.832250, 1.257570</t>
+  </si>
+  <si>
+    <t>45.895320, 1.280380</t>
+  </si>
+  <si>
+    <t>45.829520, 1.261290</t>
+  </si>
+  <si>
+    <t>45.822910, 1.218190</t>
   </si>
 </sst>
 </file>
@@ -983,8 +1046,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6676A63E-A0EC-4A87-A3BE-8F1A52F9F68C}">
   <dimension ref="A1:AI46"/>
   <sheetViews>
-    <sheetView zoomScale="96" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B22"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3849,83 +3912,163 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA0E2F95-9427-4F1A-853B-3779FAB5AD02}">
   <dimension ref="A1:G61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11:D61"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G2" sqref="G2:G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.42578125" customWidth="1"/>
+    <col min="2" max="2" width="25.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.28515625" customWidth="1"/>
     <col min="4" max="4" width="19.42578125" customWidth="1"/>
     <col min="5" max="5" width="16.85546875" customWidth="1"/>
-    <col min="6" max="6" width="17.42578125" customWidth="1"/>
+    <col min="6" max="6" width="19.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>175</v>
+      </c>
+      <c r="B1" t="s">
         <v>176</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>177</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>178</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>179</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>180</v>
-      </c>
-      <c r="F1" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
+      <c r="B2" t="s">
+        <v>184</v>
+      </c>
+      <c r="C2">
+        <v>87000</v>
+      </c>
+      <c r="D2" t="s">
+        <v>185</v>
+      </c>
+      <c r="E2" t="s">
+        <v>183</v>
+      </c>
+      <c r="F2" t="s">
+        <v>199</v>
+      </c>
       <c r="G2" t="str">
         <f>"INSERT INTO magasin (idMagasin, adresse, codePostal, description, nom, json) VALUES("&amp;A2&amp;",'"&amp;B2&amp;"',"&amp;C2&amp;",'"&amp;D2&amp;"','"&amp;E2&amp;"','"&amp;F2&amp;"');"</f>
-        <v>INSERT INTO magasin (idMagasin, adresse, codePostal, description, nom, json) VALUES(1,'',,'','','');</v>
+        <v>INSERT INTO magasin (idMagasin, adresse, codePostal, description, nom, json) VALUES(1,'26 Av. des Bénédictins',87000,'Le magasin de musique de Limoges. Une large gamme de guitares acoustiques, électriques, électro-ac mais aussi de basses, pianos, claviers et batteries.','Music Passion 87','45.832950, 1.267190');</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
+      <c r="B3" t="s">
+        <v>187</v>
+      </c>
+      <c r="C3">
+        <v>87005</v>
+      </c>
+      <c r="D3" t="s">
+        <v>188</v>
+      </c>
+      <c r="E3" t="s">
+        <v>186</v>
+      </c>
+      <c r="F3" t="s">
+        <v>200</v>
+      </c>
       <c r="G3" t="str">
         <f t="shared" ref="G3:G6" si="0">"INSERT INTO magasin (idMagasin, adresse, codePostal, description, nom, json) VALUES("&amp;A3&amp;",'"&amp;B3&amp;"',"&amp;C3&amp;",'"&amp;D3&amp;"','"&amp;E3&amp;"','"&amp;F3&amp;"');"</f>
-        <v>INSERT INTO magasin (idMagasin, adresse, codePostal, description, nom, json) VALUES(2,'',,'','','');</v>
+        <v>INSERT INTO magasin (idMagasin, adresse, codePostal, description, nom, json) VALUES(2,'8 Rue des Combes BP 30190',87005,'Située dans le centre-ville de Limoges, la Fnac vous accueille dans son magasin d’une superficie de plus de 2100m2. Vous y retrouverez tous les univers de la Fnac : livres, disques, DVD, micro‐informatique, objets connectés, gaming, téléphonie, son, photo, TV, papeterie,… Pour vos places de spectacles l’espace billetterie de Fnac Spectacles propose une large sélection d’événements.','FNAC Limoges','45.832250, 1.257570');</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
+      <c r="B4" t="s">
+        <v>190</v>
+      </c>
+      <c r="C4">
+        <v>87280</v>
+      </c>
+      <c r="D4" t="s">
+        <v>191</v>
+      </c>
+      <c r="E4" t="s">
+        <v>189</v>
+      </c>
+      <c r="F4" t="s">
+        <v>201</v>
+      </c>
       <c r="G4" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO magasin (idMagasin, adresse, codePostal, description, nom, json) VALUES(3,'',,'','','');</v>
+        <v>INSERT INTO magasin (idMagasin, adresse, codePostal, description, nom, json) VALUES(3,'30 Rue Amédée Gordini',87280,'Cultura enseigne leader de biens de loisirs culturels et créatifs','Cultura Limoges','45.895320, 1.280380');</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
+      <c r="B5" t="s">
+        <v>193</v>
+      </c>
+      <c r="C5">
+        <v>87000</v>
+      </c>
+      <c r="D5" t="s">
+        <v>194</v>
+      </c>
+      <c r="E5" t="s">
+        <v>192</v>
+      </c>
+      <c r="F5" t="s">
+        <v>202</v>
+      </c>
       <c r="G5" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO magasin (idMagasin, adresse, codePostal, description, nom, json) VALUES(4,'',,'','','');</v>
+        <v>INSERT INTO magasin (idMagasin, adresse, codePostal, description, nom, json) VALUES(4,'12 Rue Jules Guesde',87000,'Petit magasin proposant un large eventail de produits','Music Mania','45.829520, 1.261290');</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
+      <c r="B6" t="s">
+        <v>196</v>
+      </c>
+      <c r="C6">
+        <v>87000</v>
+      </c>
+      <c r="D6" t="s">
+        <v>198</v>
+      </c>
+      <c r="E6" t="s">
+        <v>197</v>
+      </c>
+      <c r="F6" t="s">
+        <v>203</v>
+      </c>
       <c r="G6" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO magasin (idMagasin, adresse, codePostal, description, nom, json) VALUES(5,'',,'','','');</v>
+        <v>INSERT INTO magasin (idMagasin, adresse, codePostal, description, nom, json) VALUES(5,'5 Rue de la Glâne',87000,'rien','Limouzik','45.822910, 1.218190');</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D8" t="s">
+        <v>195</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -3933,10 +4076,10 @@
         <v>129</v>
       </c>
       <c r="B10" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C10" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -3950,8 +4093,8 @@
         <v>5</v>
       </c>
       <c r="D11" t="str">
-        <f>"INSERT INTO lieninstrumentmagasin (idInstrument, idMagasin, stock) VALUES("&amp;A11&amp;","&amp;B11&amp;","&amp;C11&amp;");"</f>
-        <v>INSERT INTO lieninstrumentmagasin (idInstrument, idMagasin, stock) VALUES(1,1,5);</v>
+        <f>"INSERT INTO lienInstrumentMagasin (idInstrument, idMagasin, stock) VALUES("&amp;A11&amp;","&amp;B11&amp;","&amp;C11&amp;");"</f>
+        <v>INSERT INTO lienInstrumentMagasin (idInstrument, idMagasin, stock) VALUES(1,1,5);</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -3965,8 +4108,8 @@
         <v>5</v>
       </c>
       <c r="D12" t="str">
-        <f t="shared" ref="D12:D61" si="1">"INSERT INTO lieninstrumentmagasin (idInstrument, idMagasin, stock) VALUES("&amp;A12&amp;","&amp;B12&amp;","&amp;C12&amp;");"</f>
-        <v>INSERT INTO lieninstrumentmagasin (idInstrument, idMagasin, stock) VALUES(2,1,5);</v>
+        <f t="shared" ref="D12:D61" si="1">"INSERT INTO lienInstrumentMagasin (idInstrument, idMagasin, stock) VALUES("&amp;A12&amp;","&amp;B12&amp;","&amp;C12&amp;");"</f>
+        <v>INSERT INTO lienInstrumentMagasin (idInstrument, idMagasin, stock) VALUES(2,1,5);</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -3981,7 +4124,7 @@
       </c>
       <c r="D13" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO lieninstrumentmagasin (idInstrument, idMagasin, stock) VALUES(3,1,5);</v>
+        <v>INSERT INTO lienInstrumentMagasin (idInstrument, idMagasin, stock) VALUES(3,1,5);</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -3996,7 +4139,7 @@
       </c>
       <c r="D14" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO lieninstrumentmagasin (idInstrument, idMagasin, stock) VALUES(4,1,5);</v>
+        <v>INSERT INTO lienInstrumentMagasin (idInstrument, idMagasin, stock) VALUES(4,1,5);</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -4011,7 +4154,7 @@
       </c>
       <c r="D15" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO lieninstrumentmagasin (idInstrument, idMagasin, stock) VALUES(5,1,5);</v>
+        <v>INSERT INTO lienInstrumentMagasin (idInstrument, idMagasin, stock) VALUES(5,1,5);</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -4026,7 +4169,7 @@
       </c>
       <c r="D16" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO lieninstrumentmagasin (idInstrument, idMagasin, stock) VALUES(6,1,5);</v>
+        <v>INSERT INTO lienInstrumentMagasin (idInstrument, idMagasin, stock) VALUES(6,1,5);</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -4041,7 +4184,7 @@
       </c>
       <c r="D17" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO lieninstrumentmagasin (idInstrument, idMagasin, stock) VALUES(7,1,5);</v>
+        <v>INSERT INTO lienInstrumentMagasin (idInstrument, idMagasin, stock) VALUES(7,1,5);</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -4056,7 +4199,7 @@
       </c>
       <c r="D18" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO lieninstrumentmagasin (idInstrument, idMagasin, stock) VALUES(8,1,5);</v>
+        <v>INSERT INTO lienInstrumentMagasin (idInstrument, idMagasin, stock) VALUES(8,1,5);</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -4071,7 +4214,7 @@
       </c>
       <c r="D19" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO lieninstrumentmagasin (idInstrument, idMagasin, stock) VALUES(9,1,2);</v>
+        <v>INSERT INTO lienInstrumentMagasin (idInstrument, idMagasin, stock) VALUES(9,1,2);</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -4086,7 +4229,7 @@
       </c>
       <c r="D20" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO lieninstrumentmagasin (idInstrument, idMagasin, stock) VALUES(10,1,2);</v>
+        <v>INSERT INTO lienInstrumentMagasin (idInstrument, idMagasin, stock) VALUES(10,1,2);</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -4101,7 +4244,7 @@
       </c>
       <c r="D21" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO lieninstrumentmagasin (idInstrument, idMagasin, stock) VALUES(11,1,2);</v>
+        <v>INSERT INTO lienInstrumentMagasin (idInstrument, idMagasin, stock) VALUES(11,1,2);</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -4116,7 +4259,7 @@
       </c>
       <c r="D22" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO lieninstrumentmagasin (idInstrument, idMagasin, stock) VALUES(12,1,2);</v>
+        <v>INSERT INTO lienInstrumentMagasin (idInstrument, idMagasin, stock) VALUES(12,1,2);</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -4131,7 +4274,7 @@
       </c>
       <c r="D23" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO lieninstrumentmagasin (idInstrument, idMagasin, stock) VALUES(13,1,2);</v>
+        <v>INSERT INTO lienInstrumentMagasin (idInstrument, idMagasin, stock) VALUES(13,1,2);</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -4146,7 +4289,7 @@
       </c>
       <c r="D24" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO lieninstrumentmagasin (idInstrument, idMagasin, stock) VALUES(14,1,2);</v>
+        <v>INSERT INTO lienInstrumentMagasin (idInstrument, idMagasin, stock) VALUES(14,1,2);</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -4161,7 +4304,7 @@
       </c>
       <c r="D25" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO lieninstrumentmagasin (idInstrument, idMagasin, stock) VALUES(15,1,2);</v>
+        <v>INSERT INTO lienInstrumentMagasin (idInstrument, idMagasin, stock) VALUES(15,1,2);</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -4176,7 +4319,7 @@
       </c>
       <c r="D26" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO lieninstrumentmagasin (idInstrument, idMagasin, stock) VALUES(16,1,2);</v>
+        <v>INSERT INTO lienInstrumentMagasin (idInstrument, idMagasin, stock) VALUES(16,1,2);</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -4191,7 +4334,7 @@
       </c>
       <c r="D27" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO lieninstrumentmagasin (idInstrument, idMagasin, stock) VALUES(17,1,2);</v>
+        <v>INSERT INTO lienInstrumentMagasin (idInstrument, idMagasin, stock) VALUES(17,1,2);</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -4206,7 +4349,7 @@
       </c>
       <c r="D28" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO lieninstrumentmagasin (idInstrument, idMagasin, stock) VALUES(18,1,1);</v>
+        <v>INSERT INTO lienInstrumentMagasin (idInstrument, idMagasin, stock) VALUES(18,1,1);</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -4221,7 +4364,7 @@
       </c>
       <c r="D29" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO lieninstrumentmagasin (idInstrument, idMagasin, stock) VALUES(19,1,1);</v>
+        <v>INSERT INTO lienInstrumentMagasin (idInstrument, idMagasin, stock) VALUES(19,1,1);</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -4236,7 +4379,7 @@
       </c>
       <c r="D30" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO lieninstrumentmagasin (idInstrument, idMagasin, stock) VALUES(20,1,1);</v>
+        <v>INSERT INTO lienInstrumentMagasin (idInstrument, idMagasin, stock) VALUES(20,1,1);</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -4251,7 +4394,7 @@
       </c>
       <c r="D31" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO lieninstrumentmagasin (idInstrument, idMagasin, stock) VALUES(21,1,0);</v>
+        <v>INSERT INTO lienInstrumentMagasin (idInstrument, idMagasin, stock) VALUES(21,1,0);</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -4266,7 +4409,7 @@
       </c>
       <c r="D32" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO lieninstrumentmagasin (idInstrument, idMagasin, stock) VALUES(1,2,2);</v>
+        <v>INSERT INTO lienInstrumentMagasin (idInstrument, idMagasin, stock) VALUES(1,2,2);</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -4281,7 +4424,7 @@
       </c>
       <c r="D33" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO lieninstrumentmagasin (idInstrument, idMagasin, stock) VALUES(2,2,2);</v>
+        <v>INSERT INTO lienInstrumentMagasin (idInstrument, idMagasin, stock) VALUES(2,2,2);</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -4296,7 +4439,7 @@
       </c>
       <c r="D34" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO lieninstrumentmagasin (idInstrument, idMagasin, stock) VALUES(3,2,2);</v>
+        <v>INSERT INTO lienInstrumentMagasin (idInstrument, idMagasin, stock) VALUES(3,2,2);</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -4311,7 +4454,7 @@
       </c>
       <c r="D35" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO lieninstrumentmagasin (idInstrument, idMagasin, stock) VALUES(11,2,2);</v>
+        <v>INSERT INTO lienInstrumentMagasin (idInstrument, idMagasin, stock) VALUES(11,2,2);</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -4326,7 +4469,7 @@
       </c>
       <c r="D36" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO lieninstrumentmagasin (idInstrument, idMagasin, stock) VALUES(12,2,0);</v>
+        <v>INSERT INTO lienInstrumentMagasin (idInstrument, idMagasin, stock) VALUES(12,2,0);</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -4341,7 +4484,7 @@
       </c>
       <c r="D37" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO lieninstrumentmagasin (idInstrument, idMagasin, stock) VALUES(13,2,0);</v>
+        <v>INSERT INTO lienInstrumentMagasin (idInstrument, idMagasin, stock) VALUES(13,2,0);</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -4356,7 +4499,7 @@
       </c>
       <c r="D38" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO lieninstrumentmagasin (idInstrument, idMagasin, stock) VALUES(14,2,2);</v>
+        <v>INSERT INTO lienInstrumentMagasin (idInstrument, idMagasin, stock) VALUES(14,2,2);</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -4371,7 +4514,7 @@
       </c>
       <c r="D39" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO lieninstrumentmagasin (idInstrument, idMagasin, stock) VALUES(15,2,2);</v>
+        <v>INSERT INTO lienInstrumentMagasin (idInstrument, idMagasin, stock) VALUES(15,2,2);</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -4386,7 +4529,7 @@
       </c>
       <c r="D40" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO lieninstrumentmagasin (idInstrument, idMagasin, stock) VALUES(19,2,2);</v>
+        <v>INSERT INTO lienInstrumentMagasin (idInstrument, idMagasin, stock) VALUES(19,2,2);</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -4401,7 +4544,7 @@
       </c>
       <c r="D41" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO lieninstrumentmagasin (idInstrument, idMagasin, stock) VALUES(20,2,2);</v>
+        <v>INSERT INTO lienInstrumentMagasin (idInstrument, idMagasin, stock) VALUES(20,2,2);</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -4416,7 +4559,7 @@
       </c>
       <c r="D42" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO lieninstrumentmagasin (idInstrument, idMagasin, stock) VALUES(21,2,1);</v>
+        <v>INSERT INTO lienInstrumentMagasin (idInstrument, idMagasin, stock) VALUES(21,2,1);</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -4431,7 +4574,7 @@
       </c>
       <c r="D43" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO lieninstrumentmagasin (idInstrument, idMagasin, stock) VALUES(4,3,1);</v>
+        <v>INSERT INTO lienInstrumentMagasin (idInstrument, idMagasin, stock) VALUES(4,3,1);</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -4446,7 +4589,7 @@
       </c>
       <c r="D44" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO lieninstrumentmagasin (idInstrument, idMagasin, stock) VALUES(5,3,1);</v>
+        <v>INSERT INTO lienInstrumentMagasin (idInstrument, idMagasin, stock) VALUES(5,3,1);</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -4461,7 +4604,7 @@
       </c>
       <c r="D45" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO lieninstrumentmagasin (idInstrument, idMagasin, stock) VALUES(6,3,1);</v>
+        <v>INSERT INTO lienInstrumentMagasin (idInstrument, idMagasin, stock) VALUES(6,3,1);</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -4476,7 +4619,7 @@
       </c>
       <c r="D46" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO lieninstrumentmagasin (idInstrument, idMagasin, stock) VALUES(7,3,1);</v>
+        <v>INSERT INTO lienInstrumentMagasin (idInstrument, idMagasin, stock) VALUES(7,3,1);</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -4491,7 +4634,7 @@
       </c>
       <c r="D47" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO lieninstrumentmagasin (idInstrument, idMagasin, stock) VALUES(8,3,1);</v>
+        <v>INSERT INTO lienInstrumentMagasin (idInstrument, idMagasin, stock) VALUES(8,3,1);</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -4506,7 +4649,7 @@
       </c>
       <c r="D48" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO lieninstrumentmagasin (idInstrument, idMagasin, stock) VALUES(9,3,1);</v>
+        <v>INSERT INTO lienInstrumentMagasin (idInstrument, idMagasin, stock) VALUES(9,3,1);</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -4521,7 +4664,7 @@
       </c>
       <c r="D49" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO lieninstrumentmagasin (idInstrument, idMagasin, stock) VALUES(10,3,1);</v>
+        <v>INSERT INTO lienInstrumentMagasin (idInstrument, idMagasin, stock) VALUES(10,3,1);</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -4536,7 +4679,7 @@
       </c>
       <c r="D50" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO lieninstrumentmagasin (idInstrument, idMagasin, stock) VALUES(21,4,5);</v>
+        <v>INSERT INTO lienInstrumentMagasin (idInstrument, idMagasin, stock) VALUES(21,4,5);</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -4551,7 +4694,7 @@
       </c>
       <c r="D51" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO lieninstrumentmagasin (idInstrument, idMagasin, stock) VALUES(1,5,2);</v>
+        <v>INSERT INTO lienInstrumentMagasin (idInstrument, idMagasin, stock) VALUES(1,5,2);</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -4566,7 +4709,7 @@
       </c>
       <c r="D52" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO lieninstrumentmagasin (idInstrument, idMagasin, stock) VALUES(2,5,2);</v>
+        <v>INSERT INTO lienInstrumentMagasin (idInstrument, idMagasin, stock) VALUES(2,5,2);</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
@@ -4581,7 +4724,7 @@
       </c>
       <c r="D53" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO lieninstrumentmagasin (idInstrument, idMagasin, stock) VALUES(6,5,2);</v>
+        <v>INSERT INTO lienInstrumentMagasin (idInstrument, idMagasin, stock) VALUES(6,5,2);</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -4596,7 +4739,7 @@
       </c>
       <c r="D54" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO lieninstrumentmagasin (idInstrument, idMagasin, stock) VALUES(7,5,2);</v>
+        <v>INSERT INTO lienInstrumentMagasin (idInstrument, idMagasin, stock) VALUES(7,5,2);</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -4611,7 +4754,7 @@
       </c>
       <c r="D55" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO lieninstrumentmagasin (idInstrument, idMagasin, stock) VALUES(8,5,1);</v>
+        <v>INSERT INTO lienInstrumentMagasin (idInstrument, idMagasin, stock) VALUES(8,5,1);</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
@@ -4626,7 +4769,7 @@
       </c>
       <c r="D56" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO lieninstrumentmagasin (idInstrument, idMagasin, stock) VALUES(9,5,2);</v>
+        <v>INSERT INTO lienInstrumentMagasin (idInstrument, idMagasin, stock) VALUES(9,5,2);</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
@@ -4641,7 +4784,7 @@
       </c>
       <c r="D57" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO lieninstrumentmagasin (idInstrument, idMagasin, stock) VALUES(10,5,2);</v>
+        <v>INSERT INTO lienInstrumentMagasin (idInstrument, idMagasin, stock) VALUES(10,5,2);</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
@@ -4656,7 +4799,7 @@
       </c>
       <c r="D58" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO lieninstrumentmagasin (idInstrument, idMagasin, stock) VALUES(11,5,5);</v>
+        <v>INSERT INTO lienInstrumentMagasin (idInstrument, idMagasin, stock) VALUES(11,5,5);</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
@@ -4671,7 +4814,7 @@
       </c>
       <c r="D59" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO lieninstrumentmagasin (idInstrument, idMagasin, stock) VALUES(12,5,2);</v>
+        <v>INSERT INTO lienInstrumentMagasin (idInstrument, idMagasin, stock) VALUES(12,5,2);</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
@@ -4686,7 +4829,7 @@
       </c>
       <c r="D60" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO lieninstrumentmagasin (idInstrument, idMagasin, stock) VALUES(18,5,2);</v>
+        <v>INSERT INTO lienInstrumentMagasin (idInstrument, idMagasin, stock) VALUES(18,5,2);</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
@@ -4701,7 +4844,7 @@
       </c>
       <c r="D61" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO lieninstrumentmagasin (idInstrument, idMagasin, stock) VALUES(19,5,2);</v>
+        <v>INSERT INTO lienInstrumentMagasin (idInstrument, idMagasin, stock) VALUES(19,5,2);</v>
       </c>
     </row>
   </sheetData>
@@ -4714,7 +4857,7 @@
   <dimension ref="A1:F53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A43" sqref="A43:XFD43"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4952,7 +5095,7 @@
         <v>141</v>
       </c>
       <c r="E21" t="s">
-        <v>175</v>
+        <v>182</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -5760,7 +5903,7 @@
         <v>2</v>
       </c>
       <c r="E3" t="str">
-        <f t="shared" ref="E3:E25" si="1">"INSERT INTO lienAccessoireInstrument (idAccessoire, idInstrument) VALUES("&amp;D3&amp;", "&amp;A3&amp;");"</f>
+        <f t="shared" ref="E3:E23" si="1">"INSERT INTO lienAccessoireInstrument (idAccessoire, idInstrument) VALUES("&amp;D3&amp;", "&amp;A3&amp;");"</f>
         <v>INSERT INTO lienAccessoireInstrument (idAccessoire, idInstrument) VALUES(2, 2);</v>
       </c>
     </row>
@@ -7270,7 +7413,7 @@
         <v>53</v>
       </c>
       <c r="C83" t="str">
-        <f t="shared" ref="C83:C100" si="7">"INSERT INTO test.couleur (idCouleur, libelle) VALUES("&amp;A83&amp;", '"&amp;B83&amp;"');"</f>
+        <f t="shared" ref="C83:C98" si="7">"INSERT INTO test.couleur (idCouleur, libelle) VALUES("&amp;A83&amp;", '"&amp;B83&amp;"');"</f>
         <v>INSERT INTO test.couleur (idCouleur, libelle) VALUES(2, 'Carbon Grey');</v>
       </c>
     </row>

</xml_diff>